<commit_message>
Sprint Backlog updated (Sprint 1)
</commit_message>
<xml_diff>
--- a/doc/task06/SprintBacklog.xlsx
+++ b/doc/task06/SprintBacklog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dario\Documents\GitHub\ch.bfh.bti7081.s2018.white\doc\task06\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JAL\git\ch.bfh.bti7081.s2018.white\doc\task06\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{A3C6F187-CFD4-419D-8998-290D325A4D7F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9174D6F1-CBAF-401D-A280-FC77FB05E599}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14385" windowHeight="4095" tabRatio="987" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14390" windowHeight="4100" tabRatio="987" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product_Backlog" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="65">
   <si>
     <t>ID</t>
   </si>
@@ -135,39 +135,15 @@
     <t>Als Nutzer der Applikation (ungeachtet der Rolle) will ich mich über eine GUI mittels persönlichem PW und Accountname einloggen</t>
   </si>
   <si>
-    <t>Als Angehöriger will ich meine Beobachtungen zum Patient über eine GUI im Patiententagebuch erfassen können</t>
-  </si>
-  <si>
-    <t>Die Patientenbucheinträge welche durch den Angehörigen sollen dem Arzt via GUI zur Verfügung gestellt werden</t>
-  </si>
-  <si>
-    <t>Database, UI, Model, Controller</t>
-  </si>
-  <si>
     <t>Andi</t>
   </si>
   <si>
-    <t>Nick</t>
-  </si>
-  <si>
     <t>Ohran</t>
   </si>
   <si>
     <t>Janick</t>
   </si>
   <si>
-    <t>Als Arzt will ich Einträge im Angehörigentagebuch erfassen können</t>
-  </si>
-  <si>
-    <t>Als Arzt will ich meine Einträge im Angehörigentagebuch Ändern und Löschen können</t>
-  </si>
-  <si>
-    <t>Als Arzt will ich meine Angehörigentagebucheinträge den Angehörigen zugänging machen können</t>
-  </si>
-  <si>
-    <t>Als Arzt will ich den Angehörigen des Patienten die Möglichkeit geben, die geteilten Tagebucheinträge zu kommentieren</t>
-  </si>
-  <si>
     <t>Database</t>
   </si>
   <si>
@@ -192,9 +168,6 @@
     <t>Database, UI, Model, Presenter</t>
   </si>
   <si>
-    <t>Als Angehöriger will ich über eine GUI meine Einträge im Patiententagebuch jederzeit Ändern und Löschen können</t>
-  </si>
-  <si>
     <t>Presenter</t>
   </si>
   <si>
@@ -210,13 +183,52 @@
     <t>Nik</t>
   </si>
   <si>
-    <t>review</t>
-  </si>
-  <si>
     <t xml:space="preserve">Total effort done for each ID </t>
   </si>
   <si>
-    <t>Login, Datenablage, Grundaufbau der Applikation (GUI Struktur), Berechtigungsmodell, Testdaten, Sessionmanagement, dynamisches GUI (AJAX, JS etc.) etc. -&gt; wird in allen Sprints umgesetzt</t>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>NIk</t>
+  </si>
+  <si>
+    <t>Als Angehöriger will ich meine Beobachtungen zum Patient über eine GUI im Angehörigentagebuch erfassen können</t>
+  </si>
+  <si>
+    <t>Als Angehöriger will ich über eine GUI meine Einträge im Angehörigentagebuch jederzeit Löschen können</t>
+  </si>
+  <si>
+    <t>Als Angehöriger will ich über eine GUI meine Einträge im Angehörigentagebuch jederzeit Ändern können</t>
+  </si>
+  <si>
+    <t>Der behandelnde Arzt soll Angehörigentagebucheinträge kommentieren können</t>
+  </si>
+  <si>
+    <t>Als Angehöriger will ich über die Einträge im Angehörigentagebuch mit dem Arzt kommunizieren können</t>
+  </si>
+  <si>
+    <t>Die Kommentare im Angehörigetagebuch sollen vom jeweiligen Verfasser jederzeit geändert werden können</t>
+  </si>
+  <si>
+    <t>Die Kommentare im Angehörigetagebuch sollen vom jeweiligen Verfasser jederzeit gelöscht werden können</t>
+  </si>
+  <si>
+    <t>Testdaten in Datenablage generieren</t>
+  </si>
+  <si>
+    <t>Beat</t>
+  </si>
+  <si>
+    <t>Dashboard (mit Zusammenfassung der wichtigsten Informationen)</t>
+  </si>
+  <si>
+    <t>Login, Datenablage, Grundaufbau der Applikation (GUI Struktur), Berechtigungsmodell, Testdaten, Sessionmanagement, Navigation, Dashboard</t>
+  </si>
+  <si>
+    <t>Als Nutzer der Applikation will ich mittels einer übersichtlichen Menüführung durch die Applikation navigieren</t>
+  </si>
+  <si>
+    <t>Ohran, Nik</t>
   </si>
 </sst>
 </file>
@@ -273,7 +285,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -286,8 +298,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="17">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -527,11 +545,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -632,9 +663,15 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="40">
     <dxf>
@@ -759,6 +796,26 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C5700"/>
       </font>
       <fill>
@@ -769,6 +826,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -779,6 +846,36 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -809,6 +906,36 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -819,16 +946,6 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF9C5700"/>
       </font>
       <fill>
@@ -849,46 +966,6 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -934,46 +1011,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1051,7 +1088,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1350,20 +1387,20 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView zoomScale="66" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="18" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.140625" style="14" customWidth="1"/>
-    <col min="2" max="2" width="29.140625" style="2"/>
+    <col min="1" max="1" width="14.1796875" style="14" customWidth="1"/>
+    <col min="2" max="2" width="29.1796875" style="2"/>
     <col min="3" max="3" width="55" style="2"/>
-    <col min="4" max="9" width="28.140625" style="2" customWidth="1"/>
-    <col min="10" max="1025" width="11.5703125" style="2"/>
-    <col min="1026" max="16384" width="8.7109375" style="2"/>
+    <col min="4" max="9" width="28.1796875" style="2" customWidth="1"/>
+    <col min="10" max="1025" width="11.54296875" style="2"/>
+    <col min="1026" max="16384" width="8.7265625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -1389,7 +1426,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="72" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="70" x14ac:dyDescent="0.3">
       <c r="A2" s="12">
         <v>3</v>
       </c>
@@ -1411,7 +1448,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="43.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="42" x14ac:dyDescent="0.3">
       <c r="A3" s="12">
         <v>4</v>
       </c>
@@ -1433,7 +1470,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="57.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="42" x14ac:dyDescent="0.3">
       <c r="A4" s="12">
         <v>8</v>
       </c>
@@ -1441,7 +1478,7 @@
         <v>26</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D4" s="19">
         <v>0</v>
@@ -1455,7 +1492,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="29.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="28" x14ac:dyDescent="0.3">
       <c r="A5" s="12">
         <v>5</v>
       </c>
@@ -1477,7 +1514,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="72" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="56" x14ac:dyDescent="0.3">
       <c r="A6" s="12">
         <v>6</v>
       </c>
@@ -1499,7 +1536,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="57.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="56" x14ac:dyDescent="0.3">
       <c r="A7" s="12">
         <v>7</v>
       </c>
@@ -1521,7 +1558,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="100.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="84" x14ac:dyDescent="0.3">
       <c r="A8" s="12">
         <v>1</v>
       </c>
@@ -1543,7 +1580,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="87" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="84.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="13">
         <v>2</v>
       </c>
@@ -1565,7 +1602,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" ht="30.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E10" s="9">
         <f>SUM(E2:E9)</f>
         <v>210</v>
@@ -1599,20 +1636,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02FF3D15-4E8C-47CB-B190-4A3D8712E2ED}">
-  <dimension ref="A1:M14"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" zoomScale="76" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="17.42578125" style="2"/>
-    <col min="3" max="3" width="22.85546875" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="17.42578125" style="2"/>
+    <col min="1" max="2" width="17.453125" style="2"/>
+    <col min="3" max="3" width="22.81640625" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="17.453125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="3" customFormat="1" ht="48" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="3" customFormat="1" ht="47" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -1647,13 +1684,13 @@
         <v>7</v>
       </c>
       <c r="L1" s="31" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" ht="85.5" x14ac:dyDescent="0.2">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="84" x14ac:dyDescent="0.3">
       <c r="A2" s="20">
         <v>3.1</v>
       </c>
@@ -1661,13 +1698,17 @@
         <v>1</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>33</v>
+        <v>52</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
+        <v>43</v>
+      </c>
+      <c r="E2" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="F2" s="26" t="s">
+        <v>60</v>
+      </c>
       <c r="G2" s="26">
         <v>2</v>
       </c>
@@ -1677,11 +1718,11 @@
       <c r="I2" s="26"/>
       <c r="J2" s="26"/>
       <c r="K2" s="27" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="L2" s="28"/>
     </row>
-    <row r="3" spans="1:13" ht="85.5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" ht="84" x14ac:dyDescent="0.3">
       <c r="A3" s="22">
         <v>3.2</v>
       </c>
@@ -1689,27 +1730,31 @@
         <v>1</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26"/>
+        <v>43</v>
+      </c>
+      <c r="E3" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="F3" s="26" t="s">
+        <v>33</v>
+      </c>
       <c r="G3" s="26">
         <v>2</v>
       </c>
       <c r="H3" s="26">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="I3" s="26"/>
       <c r="J3" s="26"/>
       <c r="K3" s="27" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="L3" s="29"/>
     </row>
-    <row r="4" spans="1:13" ht="100.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="70.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="22">
         <v>3.3</v>
       </c>
@@ -1717,13 +1762,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>34</v>
+        <v>54</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="E4" s="26" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F4" s="26" t="s">
         <v>30</v>
@@ -1732,133 +1777,131 @@
         <v>2</v>
       </c>
       <c r="H4" s="26">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="I4" s="26"/>
       <c r="J4" s="26"/>
       <c r="K4" s="27" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="L4" s="30">
         <f>SUM(H2:H4)</f>
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="M4" s="30">
         <f>SUM(I2:I4)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="57" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" ht="70" x14ac:dyDescent="0.3">
       <c r="A5" s="22">
-        <v>4.2</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="B5" s="22">
         <v>1</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="E5" s="26" t="s">
         <v>29</v>
       </c>
       <c r="F5" s="26" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="G5" s="26">
         <v>2</v>
       </c>
       <c r="H5" s="26">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="I5" s="26"/>
       <c r="J5" s="26"/>
       <c r="K5" s="27" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="L5" s="28"/>
     </row>
-    <row r="6" spans="1:13" ht="85.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" ht="70" x14ac:dyDescent="0.3">
       <c r="A6" s="22">
-        <v>4.3</v>
+        <v>4.2</v>
       </c>
       <c r="B6" s="22">
         <v>1</v>
       </c>
       <c r="C6" s="21" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="D6" s="17" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="E6" s="26" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="F6" s="26" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G6" s="26">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H6" s="26">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I6" s="26"/>
       <c r="J6" s="26"/>
       <c r="K6" s="27" t="s">
-        <v>55</v>
-      </c>
-      <c r="L6" s="29"/>
-    </row>
-    <row r="7" spans="1:13" ht="99.75" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+      <c r="L6" s="32"/>
+    </row>
+    <row r="7" spans="1:13" ht="70" x14ac:dyDescent="0.3">
       <c r="A7" s="22">
-        <v>4.4000000000000004</v>
+        <v>4.3</v>
       </c>
       <c r="B7" s="22">
         <v>1</v>
       </c>
       <c r="C7" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="D7" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="D7" s="17" t="s">
-        <v>51</v>
-      </c>
       <c r="E7" s="26" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="F7" s="26" t="s">
-        <v>29</v>
-      </c>
-      <c r="G7" s="26">
+        <v>60</v>
+      </c>
+      <c r="G7" s="34">
+        <v>2</v>
+      </c>
+      <c r="H7" s="26">
         <v>3</v>
-      </c>
-      <c r="H7" s="26">
-        <v>6</v>
       </c>
       <c r="I7" s="26"/>
       <c r="J7" s="26"/>
-      <c r="K7" s="27" t="s">
-        <v>55</v>
-      </c>
+      <c r="K7" s="27"/>
       <c r="L7" s="32"/>
     </row>
-    <row r="8" spans="1:13" ht="72" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" ht="70.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="22">
-        <v>4.3</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="B8" s="22">
         <v>1</v>
       </c>
       <c r="C8" s="21" t="s">
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="D8" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="E8" s="26" t="s">
         <v>35</v>
-      </c>
-      <c r="E8" s="26" t="s">
-        <v>39</v>
       </c>
       <c r="F8" s="26" t="s">
         <v>30</v>
@@ -1872,18 +1915,18 @@
       <c r="I8" s="26"/>
       <c r="J8" s="26"/>
       <c r="K8" s="27" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="L8" s="30">
         <f>SUM(H5:H8)</f>
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="M8" s="30">
         <f>SUM(I5:I8)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="99.75" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" ht="84" x14ac:dyDescent="0.3">
       <c r="A9" s="22">
         <v>8.1</v>
       </c>
@@ -1894,13 +1937,13 @@
         <v>32</v>
       </c>
       <c r="D9" s="17" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="E9" s="26" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="F9" s="26" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G9" s="26">
         <v>1</v>
@@ -1909,13 +1952,15 @@
         <v>5</v>
       </c>
       <c r="I9" s="26"/>
-      <c r="J9" s="26"/>
+      <c r="J9" s="26">
+        <v>4</v>
+      </c>
       <c r="K9" s="27" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="L9" s="28"/>
     </row>
-    <row r="10" spans="1:13" ht="99.75" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" ht="84" x14ac:dyDescent="0.3">
       <c r="A10" s="22">
         <v>8.1999999999999993</v>
       </c>
@@ -1926,10 +1971,10 @@
         <v>31</v>
       </c>
       <c r="D10" s="17" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="E10" s="26" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F10" s="26" t="s">
         <v>30</v>
@@ -1943,11 +1988,11 @@
       <c r="I10" s="26"/>
       <c r="J10" s="26"/>
       <c r="K10" s="27" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="L10" s="29"/>
     </row>
-    <row r="11" spans="1:13" ht="71.25" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" ht="70" x14ac:dyDescent="0.3">
       <c r="A11" s="22">
         <v>8.3000000000000007</v>
       </c>
@@ -1955,16 +2000,16 @@
         <v>1</v>
       </c>
       <c r="C11" s="21" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="D11" s="17" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="E11" s="26" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="F11" s="26" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="G11" s="26">
         <v>0</v>
@@ -1973,13 +2018,15 @@
         <v>5</v>
       </c>
       <c r="I11" s="26"/>
-      <c r="J11" s="26"/>
+      <c r="J11" s="26">
+        <v>7</v>
+      </c>
       <c r="K11" s="27" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="L11" s="29"/>
     </row>
-    <row r="12" spans="1:13" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" ht="28" x14ac:dyDescent="0.3">
       <c r="A12" s="22">
         <v>8.4</v>
       </c>
@@ -1987,31 +2034,33 @@
         <v>1</v>
       </c>
       <c r="C12" s="21" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="D12" s="17" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="E12" s="26" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F12" s="26" t="s">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="G12" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H12" s="26">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="I12" s="26"/>
-      <c r="J12" s="26"/>
+      <c r="J12" s="26">
+        <v>3</v>
+      </c>
       <c r="K12" s="27" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="L12" s="29"/>
     </row>
-    <row r="13" spans="1:13" ht="43.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" ht="42" x14ac:dyDescent="0.3">
       <c r="A13" s="22">
         <v>8.5</v>
       </c>
@@ -2019,50 +2068,148 @@
         <v>1</v>
       </c>
       <c r="C13" s="21" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="D13" s="17" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="E13" s="26" t="s">
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="F13" s="26" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="G13" s="26">
         <v>0</v>
       </c>
       <c r="H13" s="26">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="I13" s="26"/>
       <c r="J13" s="26"/>
       <c r="K13" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="L13" s="30">
-        <f>SUM(H9:H13)</f>
-        <v>25</v>
-      </c>
-      <c r="M13" s="30">
-        <f>SUM(I9:I13)</f>
+        <v>47</v>
+      </c>
+      <c r="L13" s="29"/>
+    </row>
+    <row r="14" spans="1:13" ht="56" x14ac:dyDescent="0.3">
+      <c r="A14" s="22">
+        <v>8.6</v>
+      </c>
+      <c r="B14" s="22">
+        <v>1</v>
+      </c>
+      <c r="C14" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="D14" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="E14" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="F14" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="G14" s="26">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" ht="26.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="L14" s="33">
-        <f>SUM(L2:L13)</f>
-        <v>75</v>
-      </c>
-      <c r="M14" s="33">
-        <f>SUM(M2:M13)</f>
+      <c r="H14" s="26">
+        <v>5</v>
+      </c>
+      <c r="I14" s="26"/>
+      <c r="J14" s="26"/>
+      <c r="K14" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="L14" s="35"/>
+    </row>
+    <row r="15" spans="1:13" ht="84" x14ac:dyDescent="0.3">
+      <c r="A15" s="22">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="B15" s="22">
+        <v>1</v>
+      </c>
+      <c r="C15" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="D15" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="E15" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="F15" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="G15" s="26">
+        <v>1</v>
+      </c>
+      <c r="H15" s="26">
+        <v>3</v>
+      </c>
+      <c r="I15" s="26"/>
+      <c r="J15" s="26"/>
+      <c r="K15" s="27" t="s">
+        <v>46</v>
+      </c>
+      <c r="L15" s="35"/>
+    </row>
+    <row r="16" spans="1:13" ht="42.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="22">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="B16" s="22">
+        <v>1</v>
+      </c>
+      <c r="C16" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="E16" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="F16" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="G16" s="26">
+        <v>0</v>
+      </c>
+      <c r="H16" s="26">
+        <v>5</v>
+      </c>
+      <c r="I16" s="26"/>
+      <c r="J16" s="26">
+        <v>4</v>
+      </c>
+      <c r="K16" s="27" t="s">
+        <v>50</v>
+      </c>
+      <c r="L16" s="30">
+        <f>SUM(H9:H16)</f>
+        <v>36</v>
+      </c>
+      <c r="M16" s="30">
+        <f>SUM(I9:I16)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="12:13" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="L17" s="33">
+        <f>SUM(L2:L16)</f>
+        <v>68</v>
+      </c>
+      <c r="M17" s="33">
+        <f>SUM(M2:M16)</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:H1" xr:uid="{DC1329CF-A193-4C10-8E34-AABA2DC5005B}">
-    <sortState ref="A2:H14">
+    <sortState ref="A2:H17">
       <sortCondition ref="A1"/>
     </sortState>
   </autoFilter>
@@ -2074,61 +2221,61 @@
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L13:M13">
-    <cfRule type="cellIs" dxfId="34" priority="23" operator="lessThan">
+  <conditionalFormatting sqref="L16:M16">
+    <cfRule type="cellIs" dxfId="34" priority="5" operator="lessThan">
       <formula>45</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="21" operator="lessThan">
+    <cfRule type="cellIs" dxfId="33" priority="6" operator="greaterThan">
       <formula>45</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="20" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="32" priority="7" operator="equal">
       <formula>45</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="8" operator="lessThan">
       <formula>45</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="11" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="30" priority="9" operator="equal">
       <formula>45</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="29" priority="10" operator="lessThan">
       <formula>45</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="11" operator="greaterThan">
       <formula>45</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="8" operator="lessThan">
+    <cfRule type="cellIs" dxfId="27" priority="19" operator="equal">
       <formula>45</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="20" operator="greaterThan">
       <formula>45</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="25" priority="21" operator="lessThan">
       <formula>45</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="5" operator="lessThan">
+    <cfRule type="cellIs" dxfId="24" priority="23" operator="lessThan">
       <formula>45</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L8:M8">
-    <cfRule type="cellIs" dxfId="23" priority="22" operator="lessThan">
+    <cfRule type="cellIs" dxfId="23" priority="18" operator="lessThan">
       <formula>20</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="18" operator="lessThan">
+    <cfRule type="cellIs" dxfId="22" priority="22" operator="lessThan">
       <formula>20</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L14:M14">
-    <cfRule type="cellIs" dxfId="21" priority="4" operator="lessThan">
+  <conditionalFormatting sqref="L17:M17">
+    <cfRule type="cellIs" dxfId="21" priority="2" operator="equal">
       <formula>63</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="20" priority="3" operator="greaterThan">
       <formula>63</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="4" operator="lessThan">
       <formula>63</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G13">
+  <conditionalFormatting sqref="G2:G6">
     <cfRule type="cellIs" dxfId="18" priority="1" operator="lessThan">
       <formula>2</formula>
     </cfRule>
@@ -2143,15 +2290,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="17" operator="greaterThan" id="{635E2CEE-ED27-427B-AD79-41DFB49C9180}">
+          <x14:cfRule type="cellIs" priority="15" operator="equal" id="{8D1A8E41-E55A-4D5C-BA18-5E57E8713084}">
             <xm:f>Product_Backlog!$E$2</xm:f>
             <x14:dxf>
               <font>
-                <color rgb="FF9C0006"/>
+                <color rgb="FF9C5700"/>
               </font>
               <fill>
                 <patternFill>
-                  <bgColor rgb="FFFFC7CE"/>
+                  <bgColor rgb="FFFFEB9C"/>
                 </patternFill>
               </fill>
             </x14:dxf>
@@ -2169,8 +2316,24 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="15" operator="equal" id="{8D1A8E41-E55A-4D5C-BA18-5E57E8713084}">
+          <x14:cfRule type="cellIs" priority="17" operator="greaterThan" id="{635E2CEE-ED27-427B-AD79-41DFB49C9180}">
             <xm:f>Product_Backlog!$E$2</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF9C0006"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFFC7CE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>L4:M4</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="12" operator="equal" id="{BCFA70E4-82A5-4C26-A7AA-9C79C4CEDDC1}">
+            <xm:f>Product_Backlog!$E$3</xm:f>
             <x14:dxf>
               <font>
                 <color rgb="FF9C5700"/>
@@ -2178,22 +2341,6 @@
               <fill>
                 <patternFill>
                   <bgColor rgb="FFFFEB9C"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>L4:M4</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="14" operator="greaterThan" id="{94C6A8E7-1440-4949-88E4-D44DE9A5ED4D}">
-            <xm:f>Product_Backlog!$E$3</xm:f>
-            <x14:dxf>
-              <font>
-                <color rgb="FF9C0006"/>
-              </font>
-              <fill>
-                <patternFill>
-                  <bgColor rgb="FFFFC7CE"/>
                 </patternFill>
               </fill>
             </x14:dxf>
@@ -2211,15 +2358,15 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="12" operator="equal" id="{BCFA70E4-82A5-4C26-A7AA-9C79C4CEDDC1}">
+          <x14:cfRule type="cellIs" priority="14" operator="greaterThan" id="{94C6A8E7-1440-4949-88E4-D44DE9A5ED4D}">
             <xm:f>Product_Backlog!$E$3</xm:f>
             <x14:dxf>
               <font>
-                <color rgb="FF9C5700"/>
+                <color rgb="FF9C0006"/>
               </font>
               <fill>
                 <patternFill>
-                  <bgColor rgb="FFFFEB9C"/>
+                  <bgColor rgb="FFFFC7CE"/>
                 </patternFill>
               </fill>
             </x14:dxf>
@@ -2240,12 +2387,12 @@
       <selection sqref="A1:A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="17.42578125" style="2"/>
+    <col min="1" max="16384" width="17.453125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="3" customFormat="1" ht="47.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" s="3" customFormat="1" ht="47.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -2280,7 +2427,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" ht="13" x14ac:dyDescent="0.3">
       <c r="A2" s="10"/>
       <c r="B2" s="4"/>
       <c r="C2" s="5"/>
@@ -2293,7 +2440,7 @@
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" ht="13" x14ac:dyDescent="0.3">
       <c r="A3" s="10"/>
       <c r="B3" s="4"/>
       <c r="C3" s="5"/>
@@ -2308,7 +2455,7 @@
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" ht="13" x14ac:dyDescent="0.3">
       <c r="A4" s="10"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -2321,7 +2468,7 @@
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" ht="13" x14ac:dyDescent="0.3">
       <c r="A5" s="10"/>
       <c r="B5" s="4"/>
       <c r="C5" s="5"/>
@@ -2334,7 +2481,7 @@
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" ht="13" x14ac:dyDescent="0.3">
       <c r="A6" s="10"/>
       <c r="B6" s="4"/>
       <c r="C6" s="5"/>
@@ -2347,7 +2494,7 @@
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" ht="13" x14ac:dyDescent="0.3">
       <c r="A7" s="10"/>
       <c r="B7" s="4"/>
       <c r="C7" s="5"/>
@@ -2360,7 +2507,7 @@
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" ht="13" x14ac:dyDescent="0.3">
       <c r="A8" s="10"/>
       <c r="B8" s="4"/>
       <c r="C8" s="5"/>
@@ -2373,7 +2520,7 @@
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" ht="13" x14ac:dyDescent="0.3">
       <c r="A9" s="10"/>
       <c r="B9" s="4"/>
       <c r="C9" s="5"/>
@@ -2386,7 +2533,7 @@
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" ht="13" x14ac:dyDescent="0.3">
       <c r="A10" s="10"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -2399,7 +2546,7 @@
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" ht="13" x14ac:dyDescent="0.3">
       <c r="A11" s="10"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -2412,7 +2559,7 @@
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H12" s="2">
         <v>100</v>
       </c>
@@ -2460,12 +2607,12 @@
       <selection sqref="A1:A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="17.42578125" style="2"/>
+    <col min="1" max="16384" width="17.453125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="3" customFormat="1" ht="47.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" s="3" customFormat="1" ht="47.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -2500,7 +2647,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" ht="13" x14ac:dyDescent="0.3">
       <c r="A2" s="10"/>
       <c r="B2" s="4"/>
       <c r="C2" s="5"/>
@@ -2513,7 +2660,7 @@
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" ht="13" x14ac:dyDescent="0.3">
       <c r="A3" s="10"/>
       <c r="B3" s="4"/>
       <c r="C3" s="5"/>
@@ -2528,7 +2675,7 @@
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" ht="13" x14ac:dyDescent="0.3">
       <c r="A4" s="10"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -2541,7 +2688,7 @@
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" ht="13" x14ac:dyDescent="0.3">
       <c r="A5" s="10"/>
       <c r="B5" s="4"/>
       <c r="C5" s="5"/>
@@ -2554,7 +2701,7 @@
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" ht="13" x14ac:dyDescent="0.3">
       <c r="A6" s="10"/>
       <c r="B6" s="4"/>
       <c r="C6" s="5"/>
@@ -2567,7 +2714,7 @@
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" ht="13" x14ac:dyDescent="0.3">
       <c r="A7" s="10"/>
       <c r="B7" s="4"/>
       <c r="C7" s="5"/>
@@ -2580,7 +2727,7 @@
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" ht="13" x14ac:dyDescent="0.3">
       <c r="A8" s="10"/>
       <c r="B8" s="4"/>
       <c r="C8" s="5"/>
@@ -2593,7 +2740,7 @@
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" ht="13" x14ac:dyDescent="0.3">
       <c r="A9" s="10"/>
       <c r="B9" s="4"/>
       <c r="C9" s="5"/>
@@ -2606,7 +2753,7 @@
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" ht="13" x14ac:dyDescent="0.3">
       <c r="A10" s="10"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -2619,7 +2766,7 @@
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" ht="13" x14ac:dyDescent="0.3">
       <c r="A11" s="10"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -2632,7 +2779,7 @@
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H12" s="2">
         <v>100</v>
       </c>

</xml_diff>